<commit_message>
Data Extraction from 53 datasets of Crude Assays
</commit_message>
<xml_diff>
--- a/notebook/dataset/Basrah-Heavy-2021.xlsx
+++ b/notebook/dataset/Basrah-Heavy-2021.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Crude-Assay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\CrudeCharacterization\notebook\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7F58829-5B11-4E37-914D-787CB01DD94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F42B15-7203-4E43-907E-40A2A2F5A34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{482F5173-F057-4631-B2F3-305E20F15F6D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{482F5173-F057-4631-B2F3-305E20F15F6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Details" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Distillation" sheetId="2" r:id="rId2"/>
     <sheet name="Conventional-Results" sheetId="3" r:id="rId3"/>
     <sheet name="Property-Table" sheetId="4" r:id="rId4"/>
@@ -1537,16 +1537,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1269D4F4-38E2-483F-8ECA-735E6D62D132}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>24.2765833350037</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>23.8874954511775</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>24.0820393930906</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>50.231142131024903</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1795,12 +1795,12 @@
         <v>0.111852364526798</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>5.7335158224207499</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>11.316607675875501</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>3.6483591683687998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>8.7997789323560305</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>10.0159237151192</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>20.0337848086861</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>38.285836318049803</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>-0.96417861789857795</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>48.9158095664</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>70.364360888631794</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>13.7170391855822</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>15.9185999257859</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1912,17 +1912,17 @@
         <v>9.6862299710737894</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>17.8165939586526</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>3.6672258548598902</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>18.947246063564101</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>79.375822869340695</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>133.15309423488699</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>294.91227128116498</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>424.17791796692097</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>554.01958938553605</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>738.66967100127999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>827.43153807719204</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>976.04758877943505</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>14.3179897456064</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>64.4229037416995</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>106.054819335381</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>255.82250891424499</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>386.34725717482399</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>519.12072616835201</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>709.87783401361003</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>801.57092841313795</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>966.11189128757906</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -2104,12 +2104,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -2133,9 +2133,9 @@
       <selection activeCell="E1" sqref="E1:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>67</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>14.3179897456064</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>64.4229037416995</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>106.054819335381</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>30</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>255.82250891424499</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>50</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>386.34725717482399</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>70</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>519.12072616835201</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>90</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>709.87783401361003</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>95</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>801.57092841313795</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>100</v>
       </c>
@@ -2356,13 +2356,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E459D4EC-07C2-486D-BC52-462EA7A2E8A9}">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>67</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>1142.4220455070299</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>10.7975531966484</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>2.4565297187569902E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>-1.01325</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>-220</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>48.983296103379303</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>82.589524630850903</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>0.42898858872599799</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>0.111062899349988</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>0.94163686203411301</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>9.9307510439796705</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>89.055327874611095</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>4.31562635578343E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -3594,12 +3594,12 @@
         <v>35493.322407464002</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>98.792199646025196</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>61.889897242419799</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>68.134916081238501</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>-74.134841764092997</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -3937,9 +3937,9 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:187" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>99</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>280</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>281</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>282</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>283</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>284</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>285</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>286</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>287</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>288</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>289</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>290</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>291</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>292</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>293</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>294</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>295</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>296</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>297</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>298</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>299</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>300</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>301</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>302</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>303</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>304</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>305</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>306</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>307</v>
       </c>
@@ -7990,7 +7990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>308</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>309</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:181" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>310</v>
       </c>
@@ -8365,7 +8365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>311</v>
       </c>
@@ -8481,7 +8481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -9044,7 +9044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>313</v>
       </c>
@@ -9607,7 +9607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>314</v>
       </c>
@@ -10170,7 +10170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>315</v>
       </c>
@@ -10733,7 +10733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>316</v>
       </c>
@@ -11296,7 +11296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>317</v>
       </c>
@@ -11859,7 +11859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>318</v>
       </c>
@@ -12422,7 +12422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>319</v>
       </c>
@@ -12985,7 +12985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>320</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>321</v>
       </c>
@@ -14111,7 +14111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>322</v>
       </c>
@@ -14674,7 +14674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>323</v>
       </c>
@@ -15237,7 +15237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>324</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>325</v>
       </c>
@@ -16363,7 +16363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>326</v>
       </c>
@@ -16926,7 +16926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>327</v>
       </c>
@@ -17489,7 +17489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>328</v>
       </c>
@@ -18052,7 +18052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>329</v>
       </c>
@@ -18615,7 +18615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>330</v>
       </c>
@@ -19178,7 +19178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>331</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>332</v>
       </c>
@@ -20304,7 +20304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>333</v>
       </c>
@@ -20867,7 +20867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>334</v>
       </c>
@@ -21430,7 +21430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>335</v>
       </c>
@@ -21993,7 +21993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>336</v>
       </c>
@@ -22556,7 +22556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>337</v>
       </c>
@@ -23119,7 +23119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>338</v>
       </c>
@@ -23682,7 +23682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>339</v>
       </c>
@@ -24245,7 +24245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>340</v>
       </c>
@@ -24808,7 +24808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>341</v>
       </c>
@@ -25371,7 +25371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>342</v>
       </c>
@@ -25934,7 +25934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>343</v>
       </c>
@@ -26497,7 +26497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>344</v>
       </c>
@@ -27060,7 +27060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>345</v>
       </c>
@@ -27623,7 +27623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>346</v>
       </c>
@@ -28186,7 +28186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>347</v>
       </c>
@@ -28749,7 +28749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>348</v>
       </c>
@@ -29312,7 +29312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>349</v>
       </c>
@@ -29875,7 +29875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>350</v>
       </c>
@@ -30438,7 +30438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>351</v>
       </c>
@@ -31001,7 +31001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>352</v>
       </c>
@@ -31564,7 +31564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>353</v>
       </c>
@@ -32127,7 +32127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>354</v>
       </c>
@@ -32690,7 +32690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>355</v>
       </c>
@@ -33253,7 +33253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>356</v>
       </c>
@@ -33816,7 +33816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>357</v>
       </c>
@@ -34379,7 +34379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>358</v>
       </c>
@@ -34942,7 +34942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>359</v>
       </c>
@@ -35505,7 +35505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>360</v>
       </c>
@@ -36068,7 +36068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>361</v>
       </c>
@@ -36631,7 +36631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>362</v>
       </c>
@@ -37194,7 +37194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>363</v>
       </c>
@@ -37757,7 +37757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>364</v>
       </c>
@@ -38320,7 +38320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>365</v>
       </c>
@@ -38883,7 +38883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>366</v>
       </c>
@@ -39446,7 +39446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>367</v>
       </c>
@@ -40009,7 +40009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>368</v>
       </c>
@@ -40572,7 +40572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>369</v>
       </c>
@@ -41135,7 +41135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>370</v>
       </c>
@@ -41698,7 +41698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>371</v>
       </c>
@@ -42261,7 +42261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>372</v>
       </c>
@@ -42824,7 +42824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>373</v>
       </c>
@@ -43387,7 +43387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>374</v>
       </c>
@@ -43950,7 +43950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>375</v>
       </c>
@@ -44513,7 +44513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>376</v>
       </c>
@@ -45076,7 +45076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>377</v>
       </c>
@@ -45639,7 +45639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>378</v>
       </c>
@@ -46202,7 +46202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>379</v>
       </c>
@@ -46654,7 +46654,7 @@
         <v>36902.5480248358</v>
       </c>
     </row>
-    <row r="102" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>380</v>
       </c>
@@ -47106,7 +47106,7 @@
         <v>36593.968252914397</v>
       </c>
     </row>
-    <row r="103" spans="1:187" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>381</v>
       </c>

</xml_diff>